<commit_message>
fix overlap and update cv
</commit_message>
<xml_diff>
--- a/cv/cv.xlsx
+++ b/cv/cv.xlsx
@@ -1,27 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\mnt\tsys\repos\CV-Awesome\cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5416AD82-1B5D-4B3A-908C-CC5DF7DEE4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E3D8C9-6FD0-4190-AD79-9C5AC5A828C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
     <sheet name="training" sheetId="2" r:id="rId2"/>
     <sheet name="teaching" sheetId="3" r:id="rId3"/>
     <sheet name="research" sheetId="4" r:id="rId4"/>
-    <sheet name="research2" sheetId="8" r:id="rId5"/>
-    <sheet name="industry" sheetId="5" r:id="rId6"/>
-    <sheet name="industry2" sheetId="9" r:id="rId7"/>
-    <sheet name="leadership" sheetId="6" r:id="rId8"/>
-    <sheet name="skills" sheetId="7" r:id="rId9"/>
+    <sheet name="industry" sheetId="5" r:id="rId5"/>
+    <sheet name="leadership" sheetId="6" r:id="rId6"/>
+    <sheet name="skills" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="102">
   <si>
     <t>degree</t>
   </si>
@@ -402,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,7 +416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1237,7 +1234,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1260,7 +1257,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1329,10 +1326,30 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>2010</v>
+      </c>
+      <c r="E7">
+        <v>2010</v>
+      </c>
+      <c r="F7">
+        <v>2010</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1352,10 +1369,10 @@
         <v>2010</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1375,30 +1392,76 @@
         <v>2010</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="E10">
-        <v>2010</v>
-      </c>
-      <c r="F10">
-        <v>2010</v>
+        <v>2006</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>2005</v>
+      </c>
+      <c r="E11">
+        <v>2006</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>2005</v>
+      </c>
+      <c r="E12">
+        <v>2006</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1408,125 +1471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532BDC72-2925-49AE-B7BF-5BF1EC76F7ED}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.09765625" customWidth="1"/>
-    <col min="6" max="6" width="16.69921875" customWidth="1"/>
-    <col min="7" max="7" width="90.19921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>2005</v>
-      </c>
-      <c r="E2">
-        <v>2006</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>2005</v>
-      </c>
-      <c r="E3">
-        <v>2006</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>2005</v>
-      </c>
-      <c r="E4">
-        <v>2006</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1562,8 +1511,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1585,8 +1534,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1608,8 +1557,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1631,8 +1580,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1654,8 +1603,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1677,14 +1626,31 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1703,11 +1669,11 @@
         <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1726,11 +1692,11 @@
         <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1749,11 +1715,11 @@
         <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>75</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1772,11 +1738,11 @@
         <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1795,11 +1761,11 @@
         <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1818,30 +1784,30 @@
         <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>75</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>87</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>78</v>
+      <c r="D14">
+        <v>2006</v>
+      </c>
+      <c r="E14">
+        <v>2006</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1850,77 +1816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDAC732-C96D-49A2-B5DC-D071A2D19FBD}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>2006</v>
-      </c>
-      <c r="E2">
-        <v>2006</v>
-      </c>
-      <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1959,7 +1855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>